<commit_message>
SE-391 Renamed basynthec templates
SVN: 23859
</commit_message>
<xml_diff>
--- a/eu_basynthec/sourceTest/examples/Metabolomics-Template.xlsx
+++ b/eu_basynthec/sourceTest/examples/Metabolomics-Template.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="21105"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="21405"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="1600" windowWidth="27520" windowHeight="12740" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="openbis-metadata" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>One of mM, uM, RatioT1, or RatioCs</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+  <si>
+    <t>One of CE, ES, ME, CY, or NC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Property</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Timepoint Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>One of EX, IN, or SI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cell Location</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CompoundID</t>
+  </si>
+  <si>
+    <t>HumanReadable</t>
+  </si>
+  <si>
+    <t>Experiment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Scale</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The openBIS experiment identifier</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -30,77 +72,60 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>One of CE, ES, ME, CY, or NC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Property</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Value</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Timepoint Type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>One of EX, IN, or SI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cell Location</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CompoundID</t>
-  </si>
-  <si>
-    <t>HumanReadable</t>
-  </si>
-  <si>
-    <t>Experiment</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>Header Format</t>
+  </si>
+  <si>
+    <t>METABOL HYBRID</t>
+  </si>
+  <si>
+    <t>Must be METABOL HYBRID</t>
+  </si>
+  <si>
+    <t>Start Data Row</t>
+  </si>
+  <si>
+    <t>Start Data Col</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>The first row with data — the one that contains the column headers</t>
+  </si>
+  <si>
+    <t>The first column with data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>/TEST/TEST/TEST</t>
+  </si>
+  <si>
+    <t>EX</t>
+  </si>
+  <si>
+    <t>CE</t>
+  </si>
+  <si>
+    <t>Lin</t>
   </si>
   <si>
     <t>Strain</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Value Type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Value Unit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Scale</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The openBIS experiment identifier</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The Strain Id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>One of Value, Mean, Median, Std, Var, Error, or Iqr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -134,16 +159,44 @@
       <color indexed="23"/>
       <name val="Verdana"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Verdana"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -169,11 +222,55 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -183,8 +280,46 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="25">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -512,90 +647,125 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B2" sqref="B2:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="53" style="3" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="69.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20">
+    <row r="1" spans="1:4" ht="20">
       <c r="A1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="D1" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B4" s="5"/>
       <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B5" s="5"/>
       <c r="C5" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="B6" s="5"/>
       <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>1</v>
-      </c>
+    <row r="10" spans="1:4">
+      <c r="B10" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <colBreaks count="1" manualBreakCount="1">
     <brk id="3" max="1048575" man="1"/>
   </colBreaks>
@@ -609,30 +779,53 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:Y1"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="14" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="22" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" customWidth="1"/>
+    <col min="9" max="9" width="23" customWidth="1"/>
+    <col min="10" max="10" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
+    <row r="1" spans="1:2" s="16" customFormat="1" ht="16">
+      <c r="B1" s="16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="16" customFormat="1" ht="16">
+      <c r="B2" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="16" customFormat="1" ht="16">
+      <c r="B3" s="16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="15" customFormat="1">
+      <c r="A4" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>